<commit_message>
[DataBind] Substitutor for ExcelData
</commit_message>
<xml_diff>
--- a/selcukes-databind/src/test/resources/TestData.xlsx
+++ b/selcukes-databind/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\selcukes-excel-runner\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\selcukes-databind\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0459B4-1244-4E3D-8EE8-4454FE38BBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6601B6AB-7511-46D3-99AC-988DAEF40DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8ED8C800-1088-4943-A8AD-3DF4EB6B3031}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Screen</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Yahoo::Yahoo Login</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>${DATE}</t>
   </si>
 </sst>
 </file>
@@ -835,10 +841,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1200F9D5-93C0-4617-A842-EFDA4EEB3250}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,7 +856,7 @@
     <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -872,8 +878,11 @@
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -895,8 +904,11 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -916,8 +928,11 @@
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -936,6 +951,9 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>